<commit_message>
add numbers to excel files (card reference))
</commit_message>
<xml_diff>
--- a/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
+++ b/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moirashooter/Library/Mobile Documents/com~apple~CloudDocs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moirashooter/Desktop/PokemonTCG/BrightTide/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
   <si>
     <t>Card</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Weakness</t>
   </si>
   <si>
-    <t xml:space="preserve">2x </t>
-  </si>
-  <si>
     <t>Water</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Primarina(150) stage2 card &lt;-- Brionne</t>
   </si>
   <si>
-    <t>3x</t>
-  </si>
-  <si>
     <t>Popplio(70) Basic card</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>Retreat (energy)</t>
   </si>
   <si>
-    <t>1x</t>
-  </si>
-  <si>
     <t>Golduck(90) Stage1 &lt;-- Psyduck</t>
   </si>
   <si>
@@ -246,9 +237,6 @@
     <t>Discard up to 2 water energies from hand. This attack does 60 damage for each card you discarded in this way.</t>
   </si>
   <si>
-    <t>2x</t>
-  </si>
-  <si>
     <t>Psyduck(70) Basic</t>
   </si>
   <si>
@@ -662,12 +650,6 @@
     <t>Discard 2 cards from your hand. (If you can't discard 2 cards, you can't play this card.) Search your deck for a Pokémon, reveal it, and put it into your hand. Shuffle your deck afterward.</t>
   </si>
   <si>
-    <t>12x</t>
-  </si>
-  <si>
-    <t>8x</t>
-  </si>
-  <si>
     <t>Water Energy</t>
   </si>
   <si>
@@ -675,6 +657,81 @@
   </si>
   <si>
     <t>Lightning Energy</t>
+  </si>
+  <si>
+    <t>2x  41</t>
+  </si>
+  <si>
+    <t>2x  40</t>
+  </si>
+  <si>
+    <t>3x 39</t>
+  </si>
+  <si>
+    <t>1x 29</t>
+  </si>
+  <si>
+    <t>2x 28</t>
+  </si>
+  <si>
+    <t>1x 34</t>
+  </si>
+  <si>
+    <t>2x 37</t>
+  </si>
+  <si>
+    <t>2x 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x  33 </t>
+  </si>
+  <si>
+    <t>1x 50</t>
+  </si>
+  <si>
+    <t>2x 49</t>
+  </si>
+  <si>
+    <t>2x 53</t>
+  </si>
+  <si>
+    <t>2x 104</t>
+  </si>
+  <si>
+    <t>2x 103</t>
+  </si>
+  <si>
+    <t>2x 97</t>
+  </si>
+  <si>
+    <t>1x 116</t>
+  </si>
+  <si>
+    <t>2x 120</t>
+  </si>
+  <si>
+    <t>1x 122</t>
+  </si>
+  <si>
+    <t>2x 123</t>
+  </si>
+  <si>
+    <t>2x 127</t>
+  </si>
+  <si>
+    <t>2x 134</t>
+  </si>
+  <si>
+    <t>1x 128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x 161 </t>
+  </si>
+  <si>
+    <t>12x 166</t>
+  </si>
+  <si>
+    <t>8x 167</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,30 +1103,30 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1077,22 +1134,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1100,22 +1157,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1123,44 +1180,44 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1168,22 +1225,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1191,50 +1248,50 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
         <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1242,19 +1299,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
         <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1262,100 +1319,100 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1363,32 +1420,32 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1396,164 +1453,164 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
-        <v>71</v>
-      </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change document: add which card I need to modify, and add functions/questions
</commit_message>
<xml_diff>
--- a/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
+++ b/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
@@ -707,31 +707,31 @@
     <t>1x 116</t>
   </si>
   <si>
-    <t>2x 120</t>
-  </si>
-  <si>
-    <t>1x 122</t>
-  </si>
-  <si>
-    <t>2x 123</t>
-  </si>
-  <si>
-    <t>2x 127</t>
-  </si>
-  <si>
-    <t>2x 134</t>
-  </si>
-  <si>
-    <t>1x 128</t>
-  </si>
-  <si>
     <t>12x 166</t>
   </si>
   <si>
     <t>8x 167</t>
   </si>
   <si>
-    <t>1x 135</t>
+    <t>1x 128 py script</t>
+  </si>
+  <si>
+    <t>2x 120 v</t>
+  </si>
+  <si>
+    <t>2x 123 ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 134 ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x 122 ? </t>
+  </si>
+  <si>
+    <t>1x 135 v</t>
+  </si>
+  <si>
+    <t>2x 127 ? Heal ?</t>
   </si>
 </sst>
 </file>
@@ -1069,12 +1069,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.1640625" customWidth="1"/>
@@ -1495,7 +1496,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
@@ -1509,7 +1510,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
         <v>69</v>
@@ -1523,7 +1524,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>71</v>
@@ -1537,7 +1538,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
@@ -1551,7 +1552,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
         <v>75</v>
@@ -1565,7 +1566,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
@@ -1579,7 +1580,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
         <v>79</v>
@@ -1593,7 +1594,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
@@ -1604,7 +1605,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
check wich cards needs to be done, and add a function
</commit_message>
<xml_diff>
--- a/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
+++ b/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="460" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -704,9 +704,6 @@
     <t>2x 97</t>
   </si>
   <si>
-    <t>1x 116</t>
-  </si>
-  <si>
     <t>12x 166</t>
   </si>
   <si>
@@ -719,9 +716,6 @@
     <t>2x 120 v</t>
   </si>
   <si>
-    <t>2x 123 ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">2x 134 ? </t>
   </si>
   <si>
@@ -732,6 +726,12 @@
   </si>
   <si>
     <t>2x 127 ? Heal ?</t>
+  </si>
+  <si>
+    <t>2x 123 v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x 116 ? </t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
         <v>63</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
         <v>69</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
         <v>71</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
         <v>75</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
         <v>79</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
put some check marks, which functions is needed to work on
</commit_message>
<xml_diff>
--- a/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
+++ b/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
+    <workbookView xWindow="2720" yWindow="480" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -710,28 +710,28 @@
     <t>8x 167</t>
   </si>
   <si>
-    <t>1x 128 py script</t>
-  </si>
-  <si>
-    <t>2x 120 v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2x 134 ? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1x 122 ? </t>
-  </si>
-  <si>
-    <t>1x 135 v</t>
-  </si>
-  <si>
-    <t>2x 127 ? Heal ?</t>
-  </si>
-  <si>
-    <t>2x 123 v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1x 116 ? </t>
+    <t>1x 116 check?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 120 check ? </t>
+  </si>
+  <si>
+    <t>1x 122 check?</t>
+  </si>
+  <si>
+    <t>2x 123 check? Basic (working on it</t>
+  </si>
+  <si>
+    <t>1x 128 check? Working on damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 127 check? </t>
+  </si>
+  <si>
+    <t>2x 134 check? Function needed for flipCoin</t>
+  </si>
+  <si>
+    <t>1x 135 check?</t>
   </si>
 </sst>
 </file>
@@ -1070,12 +1070,12 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.1640625" customWidth="1"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
         <v>63</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
         <v>69</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>71</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
         <v>75</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
checked, and to do description
</commit_message>
<xml_diff>
--- a/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
+++ b/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="480" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
+    <workbookView xWindow="5580" yWindow="460" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Attack2</t>
   </si>
   <si>
-    <t>Quantatiy</t>
-  </si>
-  <si>
     <t>Weakness</t>
   </si>
   <si>
@@ -659,51 +656,6 @@
     <t>Lightning Energy</t>
   </si>
   <si>
-    <t>2x  41</t>
-  </si>
-  <si>
-    <t>2x  40</t>
-  </si>
-  <si>
-    <t>3x 39</t>
-  </si>
-  <si>
-    <t>1x 29</t>
-  </si>
-  <si>
-    <t>2x 28</t>
-  </si>
-  <si>
-    <t>1x 34</t>
-  </si>
-  <si>
-    <t>2x 37</t>
-  </si>
-  <si>
-    <t>2x 36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2x  33 </t>
-  </si>
-  <si>
-    <t>1x 50</t>
-  </si>
-  <si>
-    <t>2x 49</t>
-  </si>
-  <si>
-    <t>2x 53</t>
-  </si>
-  <si>
-    <t>2x 104</t>
-  </si>
-  <si>
-    <t>2x 103</t>
-  </si>
-  <si>
-    <t>2x 97</t>
-  </si>
-  <si>
     <t>12x 166</t>
   </si>
   <si>
@@ -728,10 +680,58 @@
     <t xml:space="preserve">2x 127 check? </t>
   </si>
   <si>
-    <t>2x 134 check? Function needed for flipCoin</t>
-  </si>
-  <si>
     <t>1x 135 check?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 134 check? </t>
+  </si>
+  <si>
+    <t>2x 37 next turn no retreat</t>
+  </si>
+  <si>
+    <t>1x 29 need work for type WATER</t>
+  </si>
+  <si>
+    <t>1x 34 # next turn less damage (20)</t>
+  </si>
+  <si>
+    <t>2x 49 right function for viewing a card?</t>
+  </si>
+  <si>
+    <t>2x 103 future damage</t>
+  </si>
+  <si>
+    <t>2x 97 check?</t>
+  </si>
+  <si>
+    <t>2x 28 check?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 36 basic pokemon ? Action = draw ? </t>
+  </si>
+  <si>
+    <t>2x  33 check?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 104 if played to evolve an pokemon ? </t>
+  </si>
+  <si>
+    <t>2x 53 discard all energy function? + prevent damage next turn</t>
+  </si>
+  <si>
+    <t>1x 50 check?</t>
+  </si>
+  <si>
+    <t>2x  41 check?</t>
+  </si>
+  <si>
+    <t>2x  40 check?</t>
+  </si>
+  <si>
+    <t>3x 39 check?</t>
+  </si>
+  <si>
+    <t>Quantatiy: ID: what do to and check?</t>
   </si>
 </sst>
 </file>
@@ -1069,9 +1069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1086,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1101,33 +1099,33 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1135,22 +1133,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1158,22 +1156,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1181,44 +1179,44 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1226,22 +1224,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
         <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1249,50 +1247,50 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
         <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1300,19 +1298,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1320,100 +1318,100 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1421,12 +1419,12 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1434,19 +1432,19 @@
         <v>97</v>
       </c>
       <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1454,7 +1452,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1462,156 +1460,156 @@
         <v>98</v>
       </c>
       <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
         <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
         <v>73</v>
-      </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
         <v>77</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
         <v>79</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
         <v>81</v>
-      </c>
-      <c r="C30" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments, need to work on
</commit_message>
<xml_diff>
--- a/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
+++ b/BrightTide/Pokemon_Card_Bright_Tide_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="460" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
+    <workbookView xWindow="13500" yWindow="460" windowWidth="22500" windowHeight="8620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,9 +677,6 @@
     <t>1x 128 check? Working on damage</t>
   </si>
   <si>
-    <t xml:space="preserve">2x 127 check? </t>
-  </si>
-  <si>
     <t>1x 135 check?</t>
   </si>
   <si>
@@ -732,6 +729,9 @@
   </si>
   <si>
     <t>Quantatiy: ID: what do to and check?</t>
+  </si>
+  <si>
+    <t>2x 127 check? Action = SELECT ? Right implementation?</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1069,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1084,7 +1086,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1110,7 +1112,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1133,7 +1135,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
@@ -1156,7 +1158,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1179,7 +1181,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -1204,7 +1206,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -1224,7 +1226,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -1252,7 +1254,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -1275,7 +1277,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -1298,7 +1300,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1318,7 +1320,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1344,7 +1346,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>42</v>
@@ -1370,7 +1372,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
@@ -1396,7 +1398,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
@@ -1429,7 +1431,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
@@ -1455,9 +1457,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
@@ -1536,7 +1538,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
         <v>72</v>
@@ -1564,7 +1566,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>76</v>
@@ -1578,7 +1580,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
         <v>78</v>

</xml_diff>